<commit_message>
fixed small mistake in excel sprint plan 4
</commit_message>
<xml_diff>
--- a/Sprint 4/Sprint_Plan.xlsx
+++ b/Sprint 4/Sprint_Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\firas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C3581F-D5C4-4C48-BCDB-C9A0E723C04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7AD668-2E3A-4FDE-A815-C228C49EAF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="1560" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -566,9 +566,6 @@
     <t>Sprint 4</t>
   </si>
   <si>
-    <t>US.17 As a developer, I want to integrate SonarQube so that I can have code analysis reports.(SP:8)</t>
-  </si>
-  <si>
     <t>Task 17.01: Create sonar-project.properties file</t>
   </si>
   <si>
@@ -723,6 +720,9 @@
   </si>
   <si>
     <t>Bug.02: As a developer, I want to fix the Instructor sign up to successfully describe whether the Instructor signed up successfully (SP:2)</t>
+  </si>
+  <si>
+    <t>US.17 As a developer, I want to integrate SonarQube so that I can have code analysis reports.(SP:20)</t>
   </si>
 </sst>
 </file>
@@ -1163,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3102,7 +3102,7 @@
     </row>
     <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="23" t="s">
-        <v>177</v>
+        <v>229</v>
       </c>
       <c r="B89" s="24"/>
       <c r="C89" s="24"/>
@@ -3117,16 +3117,16 @@
         <v>175</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C90" s="5">
         <v>5</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E90" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F90" s="12" t="s">
         <v>13</v>
@@ -3143,16 +3143,16 @@
         <v>176</v>
       </c>
       <c r="B91" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C91" s="7">
         <v>8</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E91" s="20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F91" s="14" t="s">
         <v>13</v>
@@ -3169,16 +3169,16 @@
         <v>177</v>
       </c>
       <c r="B92" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C92" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E92" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F92" s="12" t="s">
         <v>26</v>
@@ -3195,16 +3195,16 @@
         <v>179</v>
       </c>
       <c r="B93" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C93" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E93" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F93" s="14" t="s">
         <v>90</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B94" s="24"/>
       <c r="C94" s="24"/>
@@ -3233,16 +3233,16 @@
         <v>202</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C95" s="5">
         <v>3</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E95" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>13</v>
@@ -3256,7 +3256,7 @@
     </row>
     <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B96" s="24"/>
       <c r="C96" s="24"/>
@@ -3271,16 +3271,16 @@
         <v>158</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C97" s="7">
         <v>1</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E97" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F97" s="14" t="s">
         <v>90</v>
@@ -3297,16 +3297,16 @@
         <v>159</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C98" s="5">
         <v>2</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E98" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>13</v>
@@ -3323,16 +3323,16 @@
         <v>160</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C99" s="7">
         <v>1</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E99" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F99" s="14" t="s">
         <v>90</v>
@@ -3346,7 +3346,7 @@
     </row>
     <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B100" s="24"/>
       <c r="C100" s="24"/>
@@ -3361,16 +3361,16 @@
         <v>173</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C101" s="5">
         <v>2</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E101" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F101" s="12" t="s">
         <v>13</v>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B102" s="24"/>
       <c r="C102" s="24"/>
@@ -3399,16 +3399,16 @@
         <v>181</v>
       </c>
       <c r="B103" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C103" s="7">
         <v>2</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E103" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F103" s="14" t="s">
         <v>26</v>
@@ -3422,7 +3422,7 @@
     </row>
     <row r="104" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B104" s="24"/>
       <c r="C104" s="24"/>
@@ -3437,16 +3437,16 @@
         <v>183</v>
       </c>
       <c r="B105" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C105" s="5">
         <v>0</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E105" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F105" s="12" t="s">
         <v>13</v>
@@ -3463,16 +3463,16 @@
         <v>184</v>
       </c>
       <c r="B106" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C106" s="7">
         <v>2</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E106" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F106" s="14" t="s">
         <v>13</v>
@@ -3489,16 +3489,16 @@
         <v>185</v>
       </c>
       <c r="B107" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C107" s="5">
         <v>1</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E107" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F107" s="12" t="s">
         <v>13</v>
@@ -3515,16 +3515,16 @@
         <v>186</v>
       </c>
       <c r="B108" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C108" s="7">
         <v>0</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E108" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F108" s="14" t="s">
         <v>26</v>
@@ -3541,16 +3541,16 @@
         <v>187</v>
       </c>
       <c r="B109" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C109" s="5">
         <v>1</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E109" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F109" s="12" t="s">
         <v>26</v>
@@ -3567,16 +3567,16 @@
         <v>188</v>
       </c>
       <c r="B110" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C110" s="7">
         <v>1</v>
       </c>
       <c r="D110" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E110" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F110" s="14" t="s">
         <v>13</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B111" s="24"/>
       <c r="C111" s="24"/>
@@ -3605,16 +3605,16 @@
         <v>195</v>
       </c>
       <c r="B112" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C112" s="5">
         <v>1</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E112" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F112" s="12" t="s">
         <v>13</v>
@@ -3631,16 +3631,16 @@
         <v>194</v>
       </c>
       <c r="B113" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C113" s="7">
         <v>1</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E113" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F113" s="14" t="s">
         <v>26</v>
@@ -3654,7 +3654,7 @@
     </row>
     <row r="114" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B114" s="24"/>
       <c r="C114" s="24"/>
@@ -3669,16 +3669,16 @@
         <v>204</v>
       </c>
       <c r="B115" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C115" s="5">
         <v>2</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E115" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F115" s="12" t="s">
         <v>13</v>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="116" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B116" s="24"/>
       <c r="C116" s="24"/>
@@ -3707,16 +3707,16 @@
         <v>170</v>
       </c>
       <c r="B117" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C117" s="5">
         <v>1</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E117" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F117" s="12" t="s">
         <v>13</v>
@@ -3733,16 +3733,16 @@
         <v>171</v>
       </c>
       <c r="B118" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C118" s="7">
         <v>1</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E118" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F118" s="14" t="s">
         <v>26</v>
@@ -3756,7 +3756,7 @@
     </row>
     <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B119" s="24"/>
       <c r="C119" s="24"/>
@@ -3771,16 +3771,16 @@
         <v>190</v>
       </c>
       <c r="B120" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C120" s="5">
         <v>1</v>
       </c>
       <c r="D120" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E120" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F120" s="12" t="s">
         <v>13</v>
@@ -3797,16 +3797,16 @@
         <v>191</v>
       </c>
       <c r="B121" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C121" s="7">
         <v>1</v>
       </c>
       <c r="D121" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E121" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F121" s="20" t="s">
         <v>13</v>
@@ -4702,32 +4702,32 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A62:H62"/>
-    <mergeCell ref="A66:H66"/>
-    <mergeCell ref="A71:H71"/>
-    <mergeCell ref="A76:H76"/>
-    <mergeCell ref="A85:H85"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A104:H104"/>
+    <mergeCell ref="A111:H111"/>
+    <mergeCell ref="A114:H114"/>
+    <mergeCell ref="A116:H116"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="A89:H89"/>
+    <mergeCell ref="A94:H94"/>
+    <mergeCell ref="A96:H96"/>
+    <mergeCell ref="A100:H100"/>
+    <mergeCell ref="A102:H102"/>
     <mergeCell ref="A56:H56"/>
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A34:H34"/>
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="A46:H46"/>
     <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A89:H89"/>
-    <mergeCell ref="A94:H94"/>
-    <mergeCell ref="A96:H96"/>
-    <mergeCell ref="A100:H100"/>
-    <mergeCell ref="A102:H102"/>
-    <mergeCell ref="A104:H104"/>
-    <mergeCell ref="A111:H111"/>
-    <mergeCell ref="A114:H114"/>
-    <mergeCell ref="A116:H116"/>
-    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A62:H62"/>
+    <mergeCell ref="A66:H66"/>
+    <mergeCell ref="A71:H71"/>
+    <mergeCell ref="A76:H76"/>
+    <mergeCell ref="A85:H85"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="F2:G2 F4:G7 F9:G11 F13:G17 F19:G21 F23:G24 F26:G27 F36:G36 F38:G38" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>